<commit_message>
put git metadata attributes in the right order: url, branch, revision in test files; set ignore_attribute_order=True so metadata attributes in old models can be read
</commit_message>
<xml_diff>
--- a/tests/fixtures/metadata/both-metadata.xlsx
+++ b/tests/fixtures/metadata/both-metadata.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_dev_repos/obj_model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_dev_repos/obj_model/tests/fixtures/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" activeTab="3"/>
+    <workbookView xWindow="3580" yWindow="6000" windowWidth="16100" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Table of contents" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Model1s!$A$1:$A$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table of contents'!$A$1:$C$4</definedName>
   </definedNames>
-  <calcPr calcId="124519" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -650,11 +650,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="topRight" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -666,38 +666,39 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
   <dataValidations count="3">
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Branch" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Branch" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B1">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Branch" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Branch" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B2">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Revision" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Revision" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B2">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Revision" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Revision" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B3">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Url" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Url" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B3">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Url" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Url" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B1">
       <formula1>255</formula1>
     </dataValidation>
   </dataValidations>
@@ -768,7 +769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>

</xml_diff>